<commit_message>
Changed the location of the button
</commit_message>
<xml_diff>
--- a/static/purchases/purchaseHistory.xlsx
+++ b/static/purchases/purchaseHistory.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="17">
   <si>
     <t>Date</t>
   </si>
@@ -34,22 +34,10 @@
     <t>2021-04-23</t>
   </si>
   <si>
-    <t>Owain Lansdowne</t>
+    <t>Owain</t>
   </si>
   <si>
     <t>United Kingdom</t>
-  </si>
-  <si>
-    <t>11111111111111111111</t>
-  </si>
-  <si>
-    <t>Image Optim</t>
-  </si>
-  <si>
-    <t>1</t>
-  </si>
-  <si>
-    <t>Owain</t>
   </si>
   <si>
     <t>2021-03-22</t>
@@ -408,7 +396,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E14"/>
+  <dimension ref="A1:E13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -439,13 +427,10 @@
         <v>6</v>
       </c>
       <c r="C2">
-        <v>400</v>
+        <v>16500</v>
       </c>
       <c r="D2" t="s">
         <v>7</v>
-      </c>
-      <c r="E2" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -453,7 +438,7 @@
         <v>5</v>
       </c>
       <c r="B3" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="C3">
         <v>15000</v>
@@ -461,152 +446,152 @@
       <c r="D3" t="s">
         <v>7</v>
       </c>
-      <c r="E3" t="s">
-        <v>10</v>
-      </c>
     </row>
     <row r="4" spans="1:5">
       <c r="A4" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="B4" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C4">
-        <v>159500</v>
+        <v>950</v>
       </c>
       <c r="D4" t="s">
         <v>7</v>
+      </c>
+      <c r="E4" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="5" spans="1:5">
       <c r="A5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5">
+        <v>99500</v>
+      </c>
+      <c r="D5" t="s">
+        <v>7</v>
+      </c>
+      <c r="E5" t="s">
         <v>12</v>
-      </c>
-      <c r="B5" t="s">
-        <v>13</v>
-      </c>
-      <c r="C5">
-        <v>15000</v>
-      </c>
-      <c r="D5" t="s">
-        <v>7</v>
-      </c>
-      <c r="E5" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="6" spans="1:5">
       <c r="A6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6">
+        <v>16000</v>
+      </c>
+      <c r="D6" t="s">
+        <v>7</v>
+      </c>
+      <c r="E6" t="s">
         <v>12</v>
-      </c>
-      <c r="B6" t="s">
-        <v>15</v>
-      </c>
-      <c r="C6">
-        <v>30000</v>
-      </c>
-      <c r="D6" t="s">
-        <v>7</v>
-      </c>
-      <c r="E6" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="7" spans="1:5">
       <c r="A7" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="B7" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="C7">
-        <v>24500</v>
+        <v>2800</v>
       </c>
       <c r="D7" t="s">
         <v>7</v>
       </c>
       <c r="E7" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
     </row>
     <row r="8" spans="1:5">
       <c r="A8" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="B8" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="C8">
-        <v>3950</v>
+        <v>4500</v>
       </c>
       <c r="D8" t="s">
         <v>7</v>
       </c>
       <c r="E8" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
     </row>
     <row r="9" spans="1:5">
       <c r="A9" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>19</v>
+        <v>9</v>
       </c>
       <c r="C9">
-        <v>2500</v>
+        <v>15000</v>
       </c>
       <c r="D9" t="s">
         <v>7</v>
       </c>
       <c r="E9" t="s">
-        <v>20</v>
+        <v>10</v>
       </c>
     </row>
     <row r="10" spans="1:5">
       <c r="A10" t="s">
+        <v>8</v>
+      </c>
+      <c r="B10" t="s">
+        <v>11</v>
+      </c>
+      <c r="C10">
+        <v>30000</v>
+      </c>
+      <c r="D10" t="s">
+        <v>7</v>
+      </c>
+      <c r="E10" t="s">
         <v>12</v>
-      </c>
-      <c r="B10" t="s">
-        <v>13</v>
-      </c>
-      <c r="C10">
-        <v>950</v>
-      </c>
-      <c r="D10" t="s">
-        <v>7</v>
-      </c>
-      <c r="E10" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="11" spans="1:5">
       <c r="A11" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="B11" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C11">
-        <v>99500</v>
+        <v>24500</v>
       </c>
       <c r="D11" t="s">
         <v>7</v>
       </c>
       <c r="E11" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="12" spans="1:5">
       <c r="A12" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="B12" t="s">
         <v>15</v>
       </c>
       <c r="C12">
-        <v>16000</v>
+        <v>3950</v>
       </c>
       <c r="D12" t="s">
         <v>7</v>
@@ -617,36 +602,19 @@
     </row>
     <row r="13" spans="1:5">
       <c r="A13" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="B13" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C13">
-        <v>2800</v>
+        <v>2500</v>
       </c>
       <c r="D13" t="s">
         <v>7</v>
       </c>
       <c r="E13" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5">
-      <c r="A14" t="s">
-        <v>12</v>
-      </c>
-      <c r="B14" t="s">
-        <v>19</v>
-      </c>
-      <c r="C14">
-        <v>4500</v>
-      </c>
-      <c r="D14" t="s">
-        <v>7</v>
-      </c>
-      <c r="E14" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
The bar charts are working
</commit_message>
<xml_diff>
--- a/static/purchases/purchaseHistory.xlsx
+++ b/static/purchases/purchaseHistory.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="18">
   <si>
     <t>Date</t>
   </si>
@@ -31,13 +31,16 @@
     <t>Vat Number</t>
   </si>
   <si>
+    <t>2021-04-25</t>
+  </si>
+  <si>
+    <t>Owain</t>
+  </si>
+  <si>
+    <t>United Kingdom</t>
+  </si>
+  <si>
     <t>2021-04-23</t>
-  </si>
-  <si>
-    <t>Owain</t>
-  </si>
-  <si>
-    <t>United Kingdom</t>
   </si>
   <si>
     <t>2021-03-22</t>
@@ -396,7 +399,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E13"/>
+  <dimension ref="A1:E14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -427,7 +430,7 @@
         <v>6</v>
       </c>
       <c r="C2">
-        <v>15000</v>
+        <v>255000</v>
       </c>
       <c r="D2" t="s">
         <v>7</v>
@@ -435,7 +438,7 @@
     </row>
     <row r="3" spans="1:5">
       <c r="A3" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="B3" t="s">
         <v>6</v>
@@ -452,7 +455,7 @@
         <v>8</v>
       </c>
       <c r="B4" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="C4">
         <v>15000</v>
@@ -460,161 +463,175 @@
       <c r="D4" t="s">
         <v>7</v>
       </c>
-      <c r="E4" t="s">
-        <v>10</v>
-      </c>
     </row>
     <row r="5" spans="1:5">
       <c r="A5" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5">
+        <v>950</v>
+      </c>
+      <c r="D5" t="s">
+        <v>7</v>
+      </c>
+      <c r="E5" t="s">
         <v>11</v>
-      </c>
-      <c r="C5">
-        <v>30000</v>
-      </c>
-      <c r="D5" t="s">
-        <v>7</v>
-      </c>
-      <c r="E5" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="6" spans="1:5">
       <c r="A6" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6">
+        <v>99500</v>
+      </c>
+      <c r="D6" t="s">
+        <v>7</v>
+      </c>
+      <c r="E6" t="s">
         <v>13</v>
-      </c>
-      <c r="C6">
-        <v>24500</v>
-      </c>
-      <c r="D6" t="s">
-        <v>7</v>
-      </c>
-      <c r="E6" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="7" spans="1:5">
       <c r="A7" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B7" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="C7">
-        <v>3950</v>
+        <v>16000</v>
       </c>
       <c r="D7" t="s">
         <v>7</v>
       </c>
       <c r="E7" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
     </row>
     <row r="8" spans="1:5">
       <c r="A8" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B8" t="s">
+        <v>14</v>
+      </c>
+      <c r="C8">
+        <v>2800</v>
+      </c>
+      <c r="D8" t="s">
+        <v>7</v>
+      </c>
+      <c r="E8" t="s">
         <v>15</v>
-      </c>
-      <c r="C8">
-        <v>2500</v>
-      </c>
-      <c r="D8" t="s">
-        <v>7</v>
-      </c>
-      <c r="E8" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="9" spans="1:5">
       <c r="A9" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B9" t="s">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="C9">
-        <v>950</v>
+        <v>4500</v>
       </c>
       <c r="D9" t="s">
         <v>7</v>
       </c>
       <c r="E9" t="s">
-        <v>10</v>
+        <v>17</v>
       </c>
     </row>
     <row r="10" spans="1:5">
       <c r="A10" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B10" t="s">
+        <v>10</v>
+      </c>
+      <c r="C10">
+        <v>15000</v>
+      </c>
+      <c r="D10" t="s">
+        <v>7</v>
+      </c>
+      <c r="E10" t="s">
         <v>11</v>
-      </c>
-      <c r="C10">
-        <v>99500</v>
-      </c>
-      <c r="D10" t="s">
-        <v>7</v>
-      </c>
-      <c r="E10" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="11" spans="1:5">
       <c r="A11" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C11">
-        <v>16000</v>
+        <v>30000</v>
       </c>
       <c r="D11" t="s">
         <v>7</v>
       </c>
       <c r="E11" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="12" spans="1:5">
       <c r="A12" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B12" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C12">
-        <v>2800</v>
+        <v>24500</v>
       </c>
       <c r="D12" t="s">
         <v>7</v>
       </c>
       <c r="E12" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="13" spans="1:5">
       <c r="A13" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B13" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C13">
-        <v>4500</v>
+        <v>3950</v>
       </c>
       <c r="D13" t="s">
         <v>7</v>
       </c>
       <c r="E13" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5">
+      <c r="A14" t="s">
+        <v>9</v>
+      </c>
+      <c r="B14" t="s">
         <v>16</v>
+      </c>
+      <c r="C14">
+        <v>2500</v>
+      </c>
+      <c r="D14" t="s">
+        <v>7</v>
+      </c>
+      <c r="E14" t="s">
+        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added some error catching as well
</commit_message>
<xml_diff>
--- a/static/purchases/purchaseHistory.xlsx
+++ b/static/purchases/purchaseHistory.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="20">
   <si>
     <t>Date</t>
   </si>
@@ -40,34 +40,40 @@
     <t>United Kingdom</t>
   </si>
   <si>
-    <t>2021-04-23</t>
-  </si>
-  <si>
     <t>2021-03-22</t>
   </si>
   <si>
+    <t>different company</t>
+  </si>
+  <si>
+    <t>United States of America</t>
+  </si>
+  <si>
+    <t>10195882</t>
+  </si>
+  <si>
+    <t>random company</t>
+  </si>
+  <si>
+    <t>Switzerland</t>
+  </si>
+  <si>
+    <t>10194882</t>
+  </si>
+  <si>
+    <t>new company</t>
+  </si>
+  <si>
+    <t>France</t>
+  </si>
+  <si>
+    <t>10131882</t>
+  </si>
+  <si>
     <t>example company</t>
   </si>
   <si>
     <t>10191882</t>
-  </si>
-  <si>
-    <t>different company</t>
-  </si>
-  <si>
-    <t>10195882</t>
-  </si>
-  <si>
-    <t>random company</t>
-  </si>
-  <si>
-    <t>10194882</t>
-  </si>
-  <si>
-    <t>new company</t>
-  </si>
-  <si>
-    <t>10131882</t>
   </si>
 </sst>
 </file>
@@ -399,7 +405,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E14"/>
+  <dimension ref="A1:E12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -430,7 +436,7 @@
         <v>6</v>
       </c>
       <c r="C2">
-        <v>255000</v>
+        <v>950</v>
       </c>
       <c r="D2" t="s">
         <v>7</v>
@@ -441,13 +447,16 @@
         <v>8</v>
       </c>
       <c r="B3" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="C3">
-        <v>16500</v>
+        <v>30000</v>
       </c>
       <c r="D3" t="s">
-        <v>7</v>
+        <v>10</v>
+      </c>
+      <c r="E3" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -455,183 +464,152 @@
         <v>8</v>
       </c>
       <c r="B4" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="C4">
-        <v>15000</v>
+        <v>2800</v>
       </c>
       <c r="D4" t="s">
-        <v>7</v>
+        <v>13</v>
+      </c>
+      <c r="E4" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="5" spans="1:5">
       <c r="A5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B5" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="C5">
-        <v>950</v>
+        <v>4500</v>
       </c>
       <c r="D5" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="E5" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
     </row>
     <row r="6" spans="1:5">
       <c r="A6" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B6" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="C6">
-        <v>99500</v>
+        <v>950</v>
       </c>
       <c r="D6" t="s">
         <v>7</v>
       </c>
       <c r="E6" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
     </row>
     <row r="7" spans="1:5">
       <c r="A7" t="s">
+        <v>8</v>
+      </c>
+      <c r="B7" t="s">
         <v>9</v>
       </c>
-      <c r="B7" t="s">
-        <v>12</v>
-      </c>
       <c r="C7">
-        <v>16000</v>
+        <v>99500</v>
       </c>
       <c r="D7" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="E7" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="8" spans="1:5">
       <c r="A8" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8" t="s">
         <v>9</v>
       </c>
-      <c r="B8" t="s">
-        <v>14</v>
-      </c>
       <c r="C8">
-        <v>2800</v>
+        <v>16000</v>
       </c>
       <c r="D8" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="E8" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="9" spans="1:5">
       <c r="A9" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="C9">
-        <v>4500</v>
+        <v>24500</v>
       </c>
       <c r="D9" t="s">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="E9" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
     </row>
     <row r="10" spans="1:5">
       <c r="A10" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="C10">
-        <v>15000</v>
+        <v>3950</v>
       </c>
       <c r="D10" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="E10" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
     </row>
     <row r="11" spans="1:5">
       <c r="A11" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B11" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="C11">
-        <v>30000</v>
+        <v>2500</v>
       </c>
       <c r="D11" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="E11" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
     </row>
     <row r="12" spans="1:5">
       <c r="A12" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B12" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="C12">
-        <v>24500</v>
+        <v>15000</v>
       </c>
       <c r="D12" t="s">
         <v>7</v>
       </c>
       <c r="E12" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5">
-      <c r="A13" t="s">
-        <v>9</v>
-      </c>
-      <c r="B13" t="s">
-        <v>16</v>
-      </c>
-      <c r="C13">
-        <v>3950</v>
-      </c>
-      <c r="D13" t="s">
-        <v>7</v>
-      </c>
-      <c r="E13" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5">
-      <c r="A14" t="s">
-        <v>9</v>
-      </c>
-      <c r="B14" t="s">
-        <v>16</v>
-      </c>
-      <c r="C14">
-        <v>2500</v>
-      </c>
-      <c r="D14" t="s">
-        <v>7</v>
-      </c>
-      <c r="E14" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Here are the changes
</commit_message>
<xml_diff>
--- a/static/purchases/purchaseHistory.xlsx
+++ b/static/purchases/purchaseHistory.xlsx
@@ -31,7 +31,7 @@
     <t>Vat Number</t>
   </si>
   <si>
-    <t>2021-04-23</t>
+    <t>2021-04-26</t>
   </si>
   <si>
     <t>Owain</t>
@@ -427,7 +427,7 @@
         <v>6</v>
       </c>
       <c r="C2">
-        <v>15000</v>
+        <v>950</v>
       </c>
       <c r="D2" t="s">
         <v>7</v>
@@ -441,7 +441,7 @@
         <v>6</v>
       </c>
       <c r="C3">
-        <v>16500</v>
+        <v>950</v>
       </c>
       <c r="D3" t="s">
         <v>7</v>

</xml_diff>